<commit_message>
revise example data sheet to intake fetal biometry
</commit_message>
<xml_diff>
--- a/tests/data/Sydney_Python_transformation.xlsx
+++ b/tests/data/Sydney_Python_transformation.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="genotype" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="phenotype" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="severity periodicity" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="fetal_biometry" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="severity periodicity" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t xml:space="preserve">Searchable Patient ID</t>
   </si>
@@ -326,9 +327,15 @@
     <t>ZXG567</t>
   </si>
   <si>
+    <t xml:space="preserve">Tetralogy of Fallot</t>
+  </si>
+  <si>
     <t>T1</t>
   </si>
   <si>
+    <t xml:space="preserve">Type I diabetes mellitus</t>
+  </si>
+  <si>
     <t>se3453r</t>
   </si>
   <si>
@@ -338,7 +345,199 @@
     <t>E</t>
   </si>
   <si>
+    <t>Schizophrenia</t>
+  </si>
+  <si>
     <t>HP:0001250</t>
+  </si>
+  <si>
+    <t>Seizure</t>
+  </si>
+  <si>
+    <t>Donald.Duck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0002187 Large hands</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intellectual disability, profound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental deterioration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paleterx Thikarelp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">709 potato</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>Psychosis</t>
+  </si>
+  <si>
+    <t>pflanze.746</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>Delusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPD (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HC (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femur (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerebellum (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisterna Magna (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humerus (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radius (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulna (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tibia (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fibula (cm)</t>
+  </si>
+  <si>
+    <t>HC/AC</t>
+  </si>
+  <si>
+    <t>FL/AC</t>
+  </si>
+  <si>
+    <t>FL/BPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFW (g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFW Percentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHR (bpm)</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placenta Appearance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart Abnormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head Abnormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Face/Neck Abnormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spine Abnormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genitalia Normal</t>
+  </si>
+  <si>
+    <t>ID001</t>
+  </si>
+  <si>
+    <t>32w3d</t>
+  </si>
+  <si>
+    <t>Transverse</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ID002</t>
+  </si>
+  <si>
+    <t>34w0d</t>
+  </si>
+  <si>
+    <t>Cephalic</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ID003</t>
+  </si>
+  <si>
+    <t>35w1d</t>
+  </si>
+  <si>
+    <t>ID004</t>
+  </si>
+  <si>
+    <t>30w0d</t>
+  </si>
+  <si>
+    <t>Breech</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>ID005</t>
+  </si>
+  <si>
+    <t>ID006</t>
+  </si>
+  <si>
+    <t>ID007</t>
+  </si>
+  <si>
+    <t>ID008</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>ID009</t>
+  </si>
+  <si>
+    <t>ID010</t>
+  </si>
+  <si>
+    <t>ID011</t>
   </si>
   <si>
     <t xml:space="preserve">to be designed</t>
@@ -348,7 +547,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12.000000"/>
       <color theme="1"/>
@@ -461,13 +660,17 @@
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12.000000"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="18.000000"/>
+      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -812,7 +1015,7 @@
     <xf fontId="15" fillId="0" borderId="9" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
     <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -824,6 +1027,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1989,11 +2195,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B12" zoomScale="100" workbookViewId="0">
       <selection activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" style="3" width="10.83203125"/>
     <col customWidth="1" min="2" max="2" style="3" width="63.6640625"/>
@@ -2167,7 +2373,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" ht="16">
+    <row r="13" ht="21.75">
       <c r="A13" s="1" t="s">
         <v>101</v>
       </c>
@@ -2180,8 +2386,11 @@
       <c r="D13" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" ht="16">
+      <c r="E13" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" ht="21.75">
       <c r="A14" s="1" t="s">
         <v>101</v>
       </c>
@@ -2189,38 +2398,115 @@
         <v>100651</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" ht="16">
+      <c r="E14" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" ht="21.75">
       <c r="A15" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" ht="21.75">
+      <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="16" ht="16">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" ht="21.75">
+      <c r="A17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" ht="21.75">
+      <c r="A18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1268</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" ht="21.75">
+      <c r="A19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" ht="21.75">
+      <c r="A20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2235,6 +2521,1303 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>140</v>
+      </c>
+      <c r="R1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T1" t="s">
+        <v>143</v>
+      </c>
+      <c r="U1" t="s">
+        <v>144</v>
+      </c>
+      <c r="V1" t="s">
+        <v>145</v>
+      </c>
+      <c r="W1" t="s">
+        <v>146</v>
+      </c>
+      <c r="X1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2">
+        <v>8.8200000000000003</v>
+      </c>
+      <c r="D2">
+        <v>31.469999999999999</v>
+      </c>
+      <c r="E2">
+        <v>31.34</v>
+      </c>
+      <c r="F2">
+        <v>6.5899999999999999</v>
+      </c>
+      <c r="G2">
+        <v>4.4100000000000001</v>
+      </c>
+      <c r="H2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I2">
+        <v>4.9900000000000002</v>
+      </c>
+      <c r="J2">
+        <v>3.8399999999999999</v>
+      </c>
+      <c r="K2">
+        <v>4.7400000000000002</v>
+      </c>
+      <c r="L2">
+        <v>4.5700000000000003</v>
+      </c>
+      <c r="M2">
+        <v>5.04</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0.23999999999999999</v>
+      </c>
+      <c r="P2">
+        <v>0.75</v>
+      </c>
+      <c r="Q2">
+        <v>2162</v>
+      </c>
+      <c r="R2">
+        <v>46</v>
+      </c>
+      <c r="S2">
+        <v>136</v>
+      </c>
+      <c r="T2" t="s">
+        <v>152</v>
+      </c>
+      <c r="U2" t="s">
+        <v>153</v>
+      </c>
+      <c r="V2" t="s">
+        <v>154</v>
+      </c>
+      <c r="W2" t="s">
+        <v>154</v>
+      </c>
+      <c r="X2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3">
+        <v>9.2699999999999996</v>
+      </c>
+      <c r="D3">
+        <v>29.289999999999999</v>
+      </c>
+      <c r="E3">
+        <v>27.07</v>
+      </c>
+      <c r="F3">
+        <v>6.71</v>
+      </c>
+      <c r="G3">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H3">
+        <v>11.699999999999999</v>
+      </c>
+      <c r="I3">
+        <v>5.6299999999999999</v>
+      </c>
+      <c r="J3">
+        <v>4.2400000000000002</v>
+      </c>
+      <c r="K3">
+        <v>4.96</v>
+      </c>
+      <c r="L3">
+        <v>4.6200000000000001</v>
+      </c>
+      <c r="M3">
+        <v>5.3799999999999999</v>
+      </c>
+      <c r="N3">
+        <v>1.0800000000000001</v>
+      </c>
+      <c r="O3">
+        <v>0.23000000000000001</v>
+      </c>
+      <c r="P3">
+        <v>0.71999999999999997</v>
+      </c>
+      <c r="Q3">
+        <v>3333</v>
+      </c>
+      <c r="R3">
+        <v>93</v>
+      </c>
+      <c r="S3">
+        <v>150</v>
+      </c>
+      <c r="T3" t="s">
+        <v>157</v>
+      </c>
+      <c r="U3" t="s">
+        <v>153</v>
+      </c>
+      <c r="V3" t="s">
+        <v>158</v>
+      </c>
+      <c r="W3" t="s">
+        <v>158</v>
+      </c>
+      <c r="X3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4">
+        <v>8.6899999999999995</v>
+      </c>
+      <c r="D4">
+        <v>31.789999999999999</v>
+      </c>
+      <c r="E4">
+        <v>27.739999999999998</v>
+      </c>
+      <c r="F4">
+        <v>6.04</v>
+      </c>
+      <c r="G4">
+        <v>4.3700000000000001</v>
+      </c>
+      <c r="H4">
+        <v>13.6</v>
+      </c>
+      <c r="I4">
+        <v>5.6699999999999999</v>
+      </c>
+      <c r="J4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="K4">
+        <v>4.6299999999999999</v>
+      </c>
+      <c r="L4">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="M4">
+        <v>5.4400000000000004</v>
+      </c>
+      <c r="N4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="O4">
+        <v>0.23999999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="Q4">
+        <v>2058</v>
+      </c>
+      <c r="R4">
+        <v>81</v>
+      </c>
+      <c r="S4">
+        <v>121</v>
+      </c>
+      <c r="T4" t="s">
+        <v>157</v>
+      </c>
+      <c r="U4" t="s">
+        <v>153</v>
+      </c>
+      <c r="V4" t="s">
+        <v>154</v>
+      </c>
+      <c r="W4" t="s">
+        <v>158</v>
+      </c>
+      <c r="X4" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5">
+        <v>7.5099999999999998</v>
+      </c>
+      <c r="D5">
+        <v>32.140000000000001</v>
+      </c>
+      <c r="E5">
+        <v>31.460000000000001</v>
+      </c>
+      <c r="F5">
+        <v>6.8300000000000001</v>
+      </c>
+      <c r="G5">
+        <v>4.8799999999999999</v>
+      </c>
+      <c r="H5">
+        <v>10.1</v>
+      </c>
+      <c r="I5">
+        <v>5.9900000000000002</v>
+      </c>
+      <c r="J5">
+        <v>3.5600000000000001</v>
+      </c>
+      <c r="K5">
+        <v>5.1399999999999997</v>
+      </c>
+      <c r="L5">
+        <v>4.5700000000000003</v>
+      </c>
+      <c r="M5">
+        <v>4.9199999999999999</v>
+      </c>
+      <c r="N5">
+        <v>1.02</v>
+      </c>
+      <c r="O5">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P5">
+        <v>0.72999999999999998</v>
+      </c>
+      <c r="Q5">
+        <v>3573</v>
+      </c>
+      <c r="R5">
+        <v>99</v>
+      </c>
+      <c r="S5">
+        <v>139</v>
+      </c>
+      <c r="T5" t="s">
+        <v>163</v>
+      </c>
+      <c r="U5" t="s">
+        <v>164</v>
+      </c>
+      <c r="V5" t="s">
+        <v>158</v>
+      </c>
+      <c r="W5" t="s">
+        <v>158</v>
+      </c>
+      <c r="X5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6">
+        <v>8.7699999999999996</v>
+      </c>
+      <c r="D6">
+        <v>30.850000000000001</v>
+      </c>
+      <c r="E6">
+        <v>27.829999999999998</v>
+      </c>
+      <c r="F6">
+        <v>6.9400000000000004</v>
+      </c>
+      <c r="G6">
+        <v>4.46</v>
+      </c>
+      <c r="H6">
+        <v>11.199999999999999</v>
+      </c>
+      <c r="I6">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="J6">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="K6">
+        <v>4.9699999999999998</v>
+      </c>
+      <c r="L6">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="M6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="N6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O6">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P6">
+        <v>0.75</v>
+      </c>
+      <c r="Q6">
+        <v>2661</v>
+      </c>
+      <c r="R6">
+        <v>42</v>
+      </c>
+      <c r="S6">
+        <v>144</v>
+      </c>
+      <c r="T6" t="s">
+        <v>157</v>
+      </c>
+      <c r="U6" t="s">
+        <v>164</v>
+      </c>
+      <c r="V6" t="s">
+        <v>154</v>
+      </c>
+      <c r="W6" t="s">
+        <v>158</v>
+      </c>
+      <c r="X6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7">
+        <v>9.2599999999999998</v>
+      </c>
+      <c r="D7">
+        <v>30.530000000000001</v>
+      </c>
+      <c r="E7">
+        <v>31.350000000000001</v>
+      </c>
+      <c r="F7">
+        <v>5.8600000000000003</v>
+      </c>
+      <c r="G7">
+        <v>4.29</v>
+      </c>
+      <c r="H7">
+        <v>12.199999999999999</v>
+      </c>
+      <c r="I7">
+        <v>5.3099999999999996</v>
+      </c>
+      <c r="J7">
+        <v>4.6600000000000001</v>
+      </c>
+      <c r="K7">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="L7">
+        <v>4.6600000000000001</v>
+      </c>
+      <c r="M7">
+        <v>4.8700000000000001</v>
+      </c>
+      <c r="N7">
+        <v>1.02</v>
+      </c>
+      <c r="O7">
+        <v>0.23000000000000001</v>
+      </c>
+      <c r="P7">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="Q7">
+        <v>3512</v>
+      </c>
+      <c r="R7">
+        <v>95</v>
+      </c>
+      <c r="S7">
+        <v>155</v>
+      </c>
+      <c r="T7" t="s">
+        <v>152</v>
+      </c>
+      <c r="U7" t="s">
+        <v>153</v>
+      </c>
+      <c r="V7" t="s">
+        <v>154</v>
+      </c>
+      <c r="W7" t="s">
+        <v>158</v>
+      </c>
+      <c r="X7" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8">
+        <v>9.4000000000000004</v>
+      </c>
+      <c r="D8">
+        <v>29.969999999999999</v>
+      </c>
+      <c r="E8">
+        <v>28.34</v>
+      </c>
+      <c r="F8">
+        <v>6.9699999999999998</v>
+      </c>
+      <c r="G8">
+        <v>4.46</v>
+      </c>
+      <c r="H8">
+        <v>12.5</v>
+      </c>
+      <c r="I8">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="J8">
+        <v>4.6699999999999999</v>
+      </c>
+      <c r="K8">
+        <v>5.3700000000000001</v>
+      </c>
+      <c r="L8">
+        <v>4.8399999999999999</v>
+      </c>
+      <c r="M8">
+        <v>4.8300000000000001</v>
+      </c>
+      <c r="N8">
+        <v>1.0600000000000001</v>
+      </c>
+      <c r="O8">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P8">
+        <v>0.78000000000000003</v>
+      </c>
+      <c r="Q8">
+        <v>3137</v>
+      </c>
+      <c r="R8">
+        <v>65</v>
+      </c>
+      <c r="S8">
+        <v>153</v>
+      </c>
+      <c r="T8" t="s">
+        <v>163</v>
+      </c>
+      <c r="U8" t="s">
+        <v>164</v>
+      </c>
+      <c r="V8" t="s">
+        <v>154</v>
+      </c>
+      <c r="W8" t="s">
+        <v>158</v>
+      </c>
+      <c r="X8" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9">
+        <v>7.9400000000000004</v>
+      </c>
+      <c r="D9">
+        <v>30.129999999999999</v>
+      </c>
+      <c r="E9">
+        <v>28.120000000000001</v>
+      </c>
+      <c r="F9">
+        <v>6.3499999999999996</v>
+      </c>
+      <c r="G9">
+        <v>4.6799999999999997</v>
+      </c>
+      <c r="H9">
+        <v>11.4</v>
+      </c>
+      <c r="I9">
+        <v>4.9699999999999998</v>
+      </c>
+      <c r="J9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K9">
+        <v>4.9199999999999999</v>
+      </c>
+      <c r="L9">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="M9">
+        <v>4.6600000000000001</v>
+      </c>
+      <c r="N9">
+        <v>1.0700000000000001</v>
+      </c>
+      <c r="O9">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P9">
+        <v>0.77000000000000002</v>
+      </c>
+      <c r="Q9">
+        <v>2543</v>
+      </c>
+      <c r="R9">
+        <v>62</v>
+      </c>
+      <c r="S9">
+        <v>143</v>
+      </c>
+      <c r="T9" t="s">
+        <v>152</v>
+      </c>
+      <c r="U9" t="s">
+        <v>169</v>
+      </c>
+      <c r="V9" t="s">
+        <v>158</v>
+      </c>
+      <c r="W9" t="s">
+        <v>154</v>
+      </c>
+      <c r="X9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10">
+        <v>9.3399999999999999</v>
+      </c>
+      <c r="D10">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="E10">
+        <v>27.66</v>
+      </c>
+      <c r="F10">
+        <v>6.4299999999999997</v>
+      </c>
+      <c r="G10">
+        <v>4.46</v>
+      </c>
+      <c r="H10">
+        <v>10.5</v>
+      </c>
+      <c r="I10">
+        <v>4.9100000000000001</v>
+      </c>
+      <c r="J10">
+        <v>4.7400000000000002</v>
+      </c>
+      <c r="K10">
+        <v>4.8300000000000001</v>
+      </c>
+      <c r="L10">
+        <v>4.7199999999999998</v>
+      </c>
+      <c r="M10">
+        <v>5.2300000000000004</v>
+      </c>
+      <c r="N10">
+        <v>1.1899999999999999</v>
+      </c>
+      <c r="O10">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P10">
+        <v>0.70999999999999996</v>
+      </c>
+      <c r="Q10">
+        <v>3149</v>
+      </c>
+      <c r="R10">
+        <v>29</v>
+      </c>
+      <c r="S10">
+        <v>148</v>
+      </c>
+      <c r="T10" t="s">
+        <v>157</v>
+      </c>
+      <c r="U10" t="s">
+        <v>169</v>
+      </c>
+      <c r="V10" t="s">
+        <v>154</v>
+      </c>
+      <c r="W10" t="s">
+        <v>154</v>
+      </c>
+      <c r="X10" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11">
+        <v>9.25</v>
+      </c>
+      <c r="D11">
+        <v>31.690000000000001</v>
+      </c>
+      <c r="E11">
+        <v>28.140000000000001</v>
+      </c>
+      <c r="F11">
+        <v>5.6100000000000003</v>
+      </c>
+      <c r="G11">
+        <v>4.6600000000000001</v>
+      </c>
+      <c r="H11">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I11">
+        <v>5.6799999999999997</v>
+      </c>
+      <c r="J11">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="K11">
+        <v>5.0099999999999998</v>
+      </c>
+      <c r="L11">
+        <v>4.8300000000000001</v>
+      </c>
+      <c r="M11">
+        <v>5.21</v>
+      </c>
+      <c r="N11">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.23999999999999999</v>
+      </c>
+      <c r="P11">
+        <v>0.68999999999999995</v>
+      </c>
+      <c r="Q11">
+        <v>2697</v>
+      </c>
+      <c r="R11">
+        <v>41</v>
+      </c>
+      <c r="S11">
+        <v>148</v>
+      </c>
+      <c r="T11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U11" t="s">
+        <v>164</v>
+      </c>
+      <c r="V11" t="s">
+        <v>158</v>
+      </c>
+      <c r="W11" t="s">
+        <v>158</v>
+      </c>
+      <c r="X11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12">
+        <v>7.6699999999999999</v>
+      </c>
+      <c r="D12">
+        <v>31.02</v>
+      </c>
+      <c r="E12">
+        <v>29.039999999999999</v>
+      </c>
+      <c r="F12">
+        <v>5.8300000000000001</v>
+      </c>
+      <c r="G12">
+        <v>4.29</v>
+      </c>
+      <c r="H12">
+        <v>12.9</v>
+      </c>
+      <c r="I12">
+        <v>4.9699999999999998</v>
+      </c>
+      <c r="J12">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="K12">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="L12">
+        <v>5.1600000000000001</v>
+      </c>
+      <c r="M12">
+        <v>4.9900000000000002</v>
+      </c>
+      <c r="N12">
+        <v>1.0700000000000001</v>
+      </c>
+      <c r="O12">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P12">
+        <v>0.73999999999999999</v>
+      </c>
+      <c r="Q12">
+        <v>2702</v>
+      </c>
+      <c r="R12">
+        <v>34</v>
+      </c>
+      <c r="S12">
+        <v>151</v>
+      </c>
+      <c r="T12" t="s">
+        <v>152</v>
+      </c>
+      <c r="U12" t="s">
+        <v>169</v>
+      </c>
+      <c r="V12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W12" t="s">
+        <v>158</v>
+      </c>
+      <c r="X12" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13">
+        <v>8.1799999999999997</v>
+      </c>
+      <c r="D13">
+        <v>29.329999999999998</v>
+      </c>
+      <c r="E13">
+        <v>28.920000000000002</v>
+      </c>
+      <c r="F13">
+        <v>6.8499999999999996</v>
+      </c>
+      <c r="G13">
+        <v>4.21</v>
+      </c>
+      <c r="H13">
+        <v>10.699999999999999</v>
+      </c>
+      <c r="I13">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="J13">
+        <v>4.6600000000000001</v>
+      </c>
+      <c r="K13">
+        <v>5.3899999999999997</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>4.8300000000000001</v>
+      </c>
+      <c r="N13">
+        <v>1.01</v>
+      </c>
+      <c r="O13">
+        <v>0.25</v>
+      </c>
+      <c r="P13">
+        <v>0.72999999999999998</v>
+      </c>
+      <c r="Q13">
+        <v>2701</v>
+      </c>
+      <c r="R13">
+        <v>66</v>
+      </c>
+      <c r="S13">
+        <v>126</v>
+      </c>
+      <c r="T13" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" t="s">
+        <v>164</v>
+      </c>
+      <c r="V13" t="s">
+        <v>158</v>
+      </c>
+      <c r="W13" t="s">
+        <v>154</v>
+      </c>
+      <c r="X13" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14">
+        <v>8.5099999999999998</v>
+      </c>
+      <c r="D14">
+        <v>29.77</v>
+      </c>
+      <c r="E14">
+        <v>28.960000000000001</v>
+      </c>
+      <c r="F14">
+        <v>5.6600000000000001</v>
+      </c>
+      <c r="G14">
+        <v>4.46</v>
+      </c>
+      <c r="H14">
+        <v>10.9</v>
+      </c>
+      <c r="I14">
+        <v>4.9500000000000002</v>
+      </c>
+      <c r="J14">
+        <v>4.5</v>
+      </c>
+      <c r="K14">
+        <v>5.3399999999999999</v>
+      </c>
+      <c r="L14">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="M14">
+        <v>5.25</v>
+      </c>
+      <c r="N14">
+        <v>1.05</v>
+      </c>
+      <c r="O14">
+        <v>0.25</v>
+      </c>
+      <c r="P14">
+        <v>0.76000000000000001</v>
+      </c>
+      <c r="Q14">
+        <v>1874</v>
+      </c>
+      <c r="R14">
+        <v>45</v>
+      </c>
+      <c r="S14">
+        <v>153</v>
+      </c>
+      <c r="T14" t="s">
+        <v>157</v>
+      </c>
+      <c r="U14" t="s">
+        <v>164</v>
+      </c>
+      <c r="V14" t="s">
+        <v>154</v>
+      </c>
+      <c r="W14" t="s">
+        <v>154</v>
+      </c>
+      <c r="X14" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15">
+        <v>7.8200000000000003</v>
+      </c>
+      <c r="D15">
+        <v>29.41</v>
+      </c>
+      <c r="E15">
+        <v>31.370000000000001</v>
+      </c>
+      <c r="F15">
+        <v>7.1799999999999997</v>
+      </c>
+      <c r="G15">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="H15">
+        <v>11.5</v>
+      </c>
+      <c r="I15">
+        <v>5.7199999999999998</v>
+      </c>
+      <c r="J15">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K15">
+        <v>5.0300000000000002</v>
+      </c>
+      <c r="L15">
+        <v>4.5899999999999999</v>
+      </c>
+      <c r="M15">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="N15">
+        <v>0.93999999999999995</v>
+      </c>
+      <c r="O15">
+        <v>0.25</v>
+      </c>
+      <c r="P15">
+        <v>0.75</v>
+      </c>
+      <c r="Q15">
+        <v>3550</v>
+      </c>
+      <c r="R15">
+        <v>89</v>
+      </c>
+      <c r="S15">
+        <v>157</v>
+      </c>
+      <c r="T15" t="s">
+        <v>163</v>
+      </c>
+      <c r="U15" t="s">
+        <v>153</v>
+      </c>
+      <c r="V15" t="s">
+        <v>158</v>
+      </c>
+      <c r="W15" t="s">
+        <v>154</v>
+      </c>
+      <c r="X15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="D16">
+        <v>29.09</v>
+      </c>
+      <c r="E16">
+        <v>31.52</v>
+      </c>
+      <c r="F16">
+        <v>5.7000000000000002</v>
+      </c>
+      <c r="G16">
+        <v>4.6799999999999997</v>
+      </c>
+      <c r="H16">
+        <v>10.4</v>
+      </c>
+      <c r="I16">
+        <v>5.8300000000000001</v>
+      </c>
+      <c r="J16">
+        <v>4.0099999999999998</v>
+      </c>
+      <c r="K16">
+        <v>4.8399999999999999</v>
+      </c>
+      <c r="L16">
+        <v>5.3899999999999997</v>
+      </c>
+      <c r="M16">
+        <v>5.2699999999999996</v>
+      </c>
+      <c r="N16">
+        <v>0.92000000000000004</v>
+      </c>
+      <c r="O16">
+        <v>0.20999999999999999</v>
+      </c>
+      <c r="P16">
+        <v>0.79000000000000004</v>
+      </c>
+      <c r="Q16">
+        <v>1820</v>
+      </c>
+      <c r="R16">
+        <v>67</v>
+      </c>
+      <c r="S16">
+        <v>159</v>
+      </c>
+      <c r="T16" t="s">
+        <v>152</v>
+      </c>
+      <c r="U16" t="s">
+        <v>164</v>
+      </c>
+      <c r="V16" t="s">
+        <v>158</v>
+      </c>
+      <c r="W16" t="s">
+        <v>158</v>
+      </c>
+      <c r="X16" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -2242,7 +3825,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add equivalences of HGNC notations
</commit_message>
<xml_diff>
--- a/tests/data/Sydney_Python_transformation.xlsx
+++ b/tests/data/Sydney_Python_transformation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="genotype" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t xml:space="preserve">Searchable Patient ID</t>
   </si>
@@ -48,6 +48,15 @@
     <t>gene</t>
   </si>
   <si>
+    <t>Ensembl</t>
+  </si>
+  <si>
+    <t>NCBI_Gene_ID</t>
+  </si>
+  <si>
+    <t>RefSeq</t>
+  </si>
+  <si>
     <t>hgvsg</t>
   </si>
   <si>
@@ -81,6 +90,12 @@
     <t>ABCC6</t>
   </si>
   <si>
+    <t>ENSG00000091262</t>
+  </si>
+  <si>
+    <t>NM_001079528</t>
+  </si>
+  <si>
     <t>chr16:g.16177614C&gt;T</t>
   </si>
   <si>
@@ -108,6 +123,12 @@
     <t>CSMD1</t>
   </si>
   <si>
+    <t>ENSG00000183117</t>
+  </si>
+  <si>
+    <t>NM_033225</t>
+  </si>
+  <si>
     <t>chr8:g.3308452C&gt;G</t>
   </si>
   <si>
@@ -144,6 +165,12 @@
     <t>IDS</t>
   </si>
   <si>
+    <t>ENSG00000010404</t>
+  </si>
+  <si>
+    <t>NM_000202.8</t>
+  </si>
+  <si>
     <t>chrX:g.149496471C&gt;T</t>
   </si>
   <si>
@@ -162,6 +189,12 @@
     <t>ACTN3</t>
   </si>
   <si>
+    <t>ENSG00000248746</t>
+  </si>
+  <si>
+    <t>NM_001104.4</t>
+  </si>
+  <si>
     <t>chr11:g.66560624C&gt;T</t>
   </si>
   <si>
@@ -186,6 +219,12 @@
     <t>MYH3</t>
   </si>
   <si>
+    <t>ENSG00000109063</t>
+  </si>
+  <si>
+    <t>NM_002470.4</t>
+  </si>
+  <si>
     <t>chr17:g.10640399G&gt;A</t>
   </si>
   <si>
@@ -204,6 +243,12 @@
     <t>CHEK2</t>
   </si>
   <si>
+    <t>ENSG00000183765</t>
+  </si>
+  <si>
+    <t>NM_001005735.3</t>
+  </si>
+  <si>
     <t>chr22:g.28725277C&gt;T</t>
   </si>
   <si>
@@ -222,6 +267,12 @@
     <t>ATP5F1A</t>
   </si>
   <si>
+    <t>ENSG00000152234</t>
+  </si>
+  <si>
+    <t>NM_004046.6</t>
+  </si>
+  <si>
     <t>chr18:g.46084295C&gt;T</t>
   </si>
   <si>
@@ -237,6 +288,12 @@
     <t>FANCD2</t>
   </si>
   <si>
+    <t>ENSG00000144554</t>
+  </si>
+  <si>
+    <t>NM_001018115.3</t>
+  </si>
+  <si>
     <t>chr3:g.10063897G&gt;T</t>
   </si>
   <si>
@@ -252,6 +309,12 @@
     <t>DPP6</t>
   </si>
   <si>
+    <t>ENSG00000130226</t>
+  </si>
+  <si>
+    <t>NM_130797.4</t>
+  </si>
+  <si>
     <t>chr7:g.153887732A&gt;C</t>
   </si>
   <si>
@@ -262,6 +325,12 @@
   </si>
   <si>
     <t>KIF4A</t>
+  </si>
+  <si>
+    <t>ENSG00000090889</t>
+  </si>
+  <si>
+    <t>NM_012310.5</t>
   </si>
   <si>
     <t>chrX:g.70290790A&gt;G</t>
@@ -547,7 +616,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20">
+  <fonts count="24">
     <font>
       <sz val="12.000000"/>
       <color theme="1"/>
@@ -659,6 +728,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="8.500000"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.000000"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.500000"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="12.000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -670,7 +760,6 @@
     </font>
     <font>
       <sz val="18.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1015,8 +1104,11 @@
     <xf fontId="15" fillId="0" borderId="9" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyProtection="0"/>
     <xf fontId="16" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1026,8 +1118,35 @@
     <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="17" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="23" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1589,7 +1708,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="120" workbookViewId="0">
       <selection activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1601,12 +1720,13 @@
     <col min="4" max="6" style="1" width="10.83203125"/>
     <col customWidth="1" min="7" max="8" style="1" width="5.83203125"/>
     <col min="9" max="9" style="1" width="10.83203125"/>
-    <col customWidth="1" min="10" max="10" style="1" width="19.83203125"/>
-    <col customWidth="1" min="11" max="11" style="1" width="28.83203125"/>
-    <col customWidth="1" min="12" max="12" style="1" width="29.1640625"/>
-    <col customWidth="1" min="13" max="14" style="1" width="33.5"/>
-    <col customWidth="1" min="15" max="15" style="1" width="15.1640625"/>
-    <col min="16" max="16384" style="1" width="10.83203125"/>
+    <col min="10" max="12" style="1" width="10.83203125"/>
+    <col customWidth="1" min="13" max="13" style="1" width="19.83203125"/>
+    <col customWidth="1" min="14" max="14" style="1" width="28.83203125"/>
+    <col customWidth="1" min="15" max="15" style="1" width="29.1640625"/>
+    <col customWidth="1" min="16" max="17" style="1" width="33.5"/>
+    <col customWidth="1" min="18" max="18" style="1" width="15.1640625"/>
+    <col min="19" max="16384" style="1" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1637,13 +1757,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1654,6 +1774,15 @@
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -1661,10 +1790,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1">
         <v>16177613</v>
@@ -1673,31 +1802,40 @@
         <v>16177614</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1">
+        <v>368</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -1705,10 +1843,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1">
         <v>3308451</v>
@@ -1717,31 +1855,40 @@
         <v>3308452</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4">
+        <v>64478</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4">
@@ -1749,10 +1896,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1">
         <v>3586228</v>
@@ -1761,31 +1908,40 @@
         <v>3586229</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="4">
+        <v>64478</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5">
@@ -1793,10 +1949,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1">
         <v>149496470</v>
@@ -1805,31 +1961,40 @@
         <v>149496471</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3423</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -1837,10 +2002,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E6" s="1">
         <v>66560623</v>
@@ -1849,31 +2014,40 @@
         <v>66560624</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="4">
+        <v>89</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -1881,10 +2055,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1">
         <v>10640398</v>
@@ -1893,31 +2067,40 @@
         <v>10640399</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4621</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -1925,43 +2108,52 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="7">
         <v>28725276</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="7">
         <v>28725277</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>58</v>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="7">
+        <v>11200</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9">
@@ -1969,10 +2161,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1">
         <v>46084294</v>
@@ -1981,31 +2173,40 @@
         <v>46084295</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="4">
+        <v>498</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>34</v>
+        <v>86</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10">
@@ -2013,10 +2214,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E10" s="1">
         <v>10063896</v>
@@ -2025,31 +2226,40 @@
         <v>10063897</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2177</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>34</v>
+        <v>93</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -2057,10 +2267,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E11">
         <v>153887731</v>
@@ -2069,31 +2279,40 @@
         <v>153887732</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" t="s">
-        <v>77</v>
-      </c>
-      <c r="K11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L11" t="s">
-        <v>79</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>58</v>
+        <v>95</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="9">
+        <v>1804</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" t="s">
+        <v>99</v>
+      </c>
+      <c r="O11" t="s">
+        <v>100</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12">
@@ -2101,10 +2320,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <v>70290789</v>
@@ -2113,31 +2332,40 @@
         <v>70290790</v>
       </c>
       <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="9">
+        <v>24137</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+      <c r="N12" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12" t="s">
+        <v>106</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" t="s">
-        <v>81</v>
-      </c>
-      <c r="K12" t="s">
-        <v>82</v>
-      </c>
-      <c r="L12" t="s">
-        <v>83</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>58</v>
+      <c r="Q12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13">
@@ -2145,10 +2373,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E13">
         <v>70290789</v>
@@ -2157,31 +2385,40 @@
         <v>70290790</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" t="s">
-        <v>82</v>
-      </c>
-      <c r="L13" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>58</v>
+        <v>101</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="9">
+        <v>24137</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" t="s">
+        <v>106</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2201,312 +2438,312 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="3" width="10.83203125"/>
-    <col customWidth="1" min="2" max="2" style="3" width="63.6640625"/>
-    <col min="3" max="3" style="3" width="10.83203125"/>
-    <col customWidth="1" min="4" max="4" style="3" width="23.33203125"/>
-    <col min="5" max="16384" style="3" width="10.83203125"/>
+    <col min="1" max="1" style="13" width="10.83203125"/>
+    <col customWidth="1" min="2" max="2" style="13" width="63.6640625"/>
+    <col min="3" max="3" style="13" width="10.83203125"/>
+    <col customWidth="1" min="4" max="4" style="13" width="23.33203125"/>
+    <col min="5" max="16384" style="13" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>87</v>
+      <c r="A1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>90</v>
+      <c r="B2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>90</v>
+      <c r="B3" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>90</v>
+      <c r="B4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>90</v>
+      <c r="B5" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>90</v>
+      <c r="B6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>90</v>
+      <c r="B7" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>90</v>
+      <c r="B8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>90</v>
+      <c r="B9" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>90</v>
+      <c r="B10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>90</v>
+      <c r="B11" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>89</v>
+      <c r="B12" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="13" ht="21.75">
       <c r="A13" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B13" s="1">
         <v>1636</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>102</v>
+        <v>113</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="14" ht="21.75">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B14" s="1">
         <v>100651</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" ht="21.75">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>108</v>
+        <v>130</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16" ht="21.75">
       <c r="A16" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>110</v>
+        <v>130</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="17" ht="21.75">
-      <c r="A17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>115</v>
+      <c r="A17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="18" ht="21.75">
-      <c r="A18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="A18" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="13">
         <v>1268</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>116</v>
+      <c r="C18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="19" ht="21.75">
-      <c r="A19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>120</v>
+      <c r="A19" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="20" ht="21.75">
-      <c r="A20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>124</v>
+      <c r="A20" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2528,90 +2765,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="I1" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="J1" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="K1" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="L1" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="M1" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="N1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="O1" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="P1" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="Q1" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="R1" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="S1" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="T1" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="U1" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="V1" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="W1" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="X1" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="Y1" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="Z1" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C2">
         <v>8.8200000000000003</v>
@@ -2665,33 +2902,33 @@
         <v>136</v>
       </c>
       <c r="T2" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="U2" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="V2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Y2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z2" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C3">
         <v>9.2699999999999996</v>
@@ -2745,33 +2982,33 @@
         <v>150</v>
       </c>
       <c r="T3" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="U3" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="V3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z3" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="C4">
         <v>8.6899999999999995</v>
@@ -2825,33 +3062,33 @@
         <v>121</v>
       </c>
       <c r="T4" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="U4" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="V4" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W4" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X4" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y4" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z4" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C5">
         <v>7.5099999999999998</v>
@@ -2905,33 +3142,33 @@
         <v>139</v>
       </c>
       <c r="T5" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="U5" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V5" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W5" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X5" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y5" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z5" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C6">
         <v>8.7699999999999996</v>
@@ -2985,33 +3222,33 @@
         <v>144</v>
       </c>
       <c r="T6" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="U6" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V6" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W6" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X6" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Y6" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z6" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C7">
         <v>9.2599999999999998</v>
@@ -3065,33 +3302,33 @@
         <v>155</v>
       </c>
       <c r="T7" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="U7" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="V7" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W7" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X7" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y7" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z7" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C8">
         <v>9.4000000000000004</v>
@@ -3145,33 +3382,33 @@
         <v>153</v>
       </c>
       <c r="T8" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="U8" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V8" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W8" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X8" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y8" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z8" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="C9">
         <v>7.9400000000000004</v>
@@ -3225,33 +3462,33 @@
         <v>143</v>
       </c>
       <c r="T9" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="U9" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="V9" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W9" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X9" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y9" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z9" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C10">
         <v>9.3399999999999999</v>
@@ -3305,33 +3542,33 @@
         <v>148</v>
       </c>
       <c r="T10" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="U10" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="V10" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W10" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X10" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y10" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z10" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C11">
         <v>9.25</v>
@@ -3385,33 +3622,33 @@
         <v>148</v>
       </c>
       <c r="T11" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="U11" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V11" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W11" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X11" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y11" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z11" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C12">
         <v>7.6699999999999999</v>
@@ -3465,33 +3702,33 @@
         <v>151</v>
       </c>
       <c r="T12" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="U12" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="V12" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W12" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X12" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y12" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z12" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C13">
         <v>8.1799999999999997</v>
@@ -3545,33 +3782,33 @@
         <v>126</v>
       </c>
       <c r="T13" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="U13" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V13" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W13" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X13" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Y13" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z13" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C14">
         <v>8.5099999999999998</v>
@@ -3625,33 +3862,33 @@
         <v>153</v>
       </c>
       <c r="T14" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="U14" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V14" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="W14" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X14" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Y14" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z14" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>111</v>
+      <c r="A15" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="C15">
         <v>7.8200000000000003</v>
@@ -3705,33 +3942,33 @@
         <v>157</v>
       </c>
       <c r="T15" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="U15" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="V15" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W15" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="X15" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Y15" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Z15" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>117</v>
+      <c r="A16" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="C16">
         <v>9.0500000000000007</v>
@@ -3785,25 +4022,25 @@
         <v>159</v>
       </c>
       <c r="T16" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="U16" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="V16" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="W16" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="X16" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="Y16" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="Z16" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3825,7 +4062,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>